<commit_message>
[Plan] Update the start time
</commit_message>
<xml_diff>
--- a/BookList.xlsx
+++ b/BookList.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="大杂烩" sheetId="1" r:id="rId1"/>
     <sheet name="C++" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="C" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Book Name</t>
   </si>
@@ -65,6 +65,14 @@
   </si>
   <si>
     <t>软件开发者路线图：从学徒到高手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ongoing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backlog</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -133,7 +141,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -141,6 +149,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -446,7 +457,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -477,55 +488,91 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="3">
+        <v>42534</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>10</v>
       </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>

</xml_diff>

<commit_message>
[Plan] Upgrade book plan and write the note
</commit_message>
<xml_diff>
--- a/BookList.xlsx
+++ b/BookList.xlsx
@@ -11,12 +11,12 @@
     <sheet name="C++" sheetId="2" r:id="rId2"/>
     <sheet name="C" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Book Name</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>程序员修炼之道</t>
-  </si>
-  <si>
     <t>程序员的自我修养</t>
   </si>
   <si>
@@ -74,43 +71,76 @@
   <si>
     <t>Backlog</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重构：改善既有代码的设计</t>
+  </si>
+  <si>
+    <t>设计模式：可复用面向对象软件的基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effective C++</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改代码的艺术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Second</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Third</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>书不是很厚，第一次用了两个多小时的时间看完了。看完后没什么好大的感触，我决定看下一本书，然后看看能不能联系起来。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>程序员修炼之道：从小工到专家</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF002060"/>
+      <color indexed="56"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF002060"/>
+      <color indexed="56"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -122,7 +152,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor indexed="17"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,7 +171,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -154,22 +184,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FF802DFB"/>
-    </mruColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -453,126 +487,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D12"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="41.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" s="3">
+        <v>42533.887835648151</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3">
-        <v>42534</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42533.91815972222</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -584,11 +644,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -614,7 +674,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>